<commit_message>
updated ALUM path in workflows
</commit_message>
<xml_diff>
--- a/NeapWorkflow GET_MarineTerrestrial_Extant-2020_250m.xlsx
+++ b/NeapWorkflow GET_MarineTerrestrial_Extant-2020_250m.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{0DDCB378-37A0-4C7E-A94E-D99B90618828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5829E69D-188E-47D1-89EB-22EA3ECCC4A5}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{0DDCB378-37A0-4C7E-A94E-D99B90618828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EFC1B9B-D556-4270-842C-2D22BDB2BB5E}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="23016" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19428" yWindow="0" windowWidth="22740" windowHeight="18744" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -177,10 +177,10 @@
     <t>ALUM_2020-IUCNGET</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\ALUM_2020_EPSG3577_250m.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
   </si>
 </sst>
 </file>
@@ -533,13 +533,13 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="221.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
@@ -762,8 +762,8 @@
       <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
-        <v>50</v>
+      <c r="B7" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -784,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -805,8 +805,9 @@
     <hyperlink ref="I4" r:id="rId8" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
     <hyperlink ref="B4" r:id="rId9" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
     <hyperlink ref="I7" r:id="rId10" xr:uid="{612F4191-C4AF-421A-86E9-1939EAAA68F6}"/>
+    <hyperlink ref="B7" r:id="rId11" xr:uid="{ECF0F928-1915-4CD2-88E1-C8D7F89239D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>